<commit_message>
prep lista de chamadas 2
</commit_message>
<xml_diff>
--- a/Lista de Presença - Outros Eventos.xlsx
+++ b/Lista de Presença - Outros Eventos.xlsx
@@ -542,7 +542,7 @@
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K2" t="n">
         <v>0.25</v>
@@ -934,7 +934,7 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K9" t="n">
         <v>0.25</v>
@@ -1102,7 +1102,7 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="K12" t="n">
         <v>-0.25</v>
@@ -1158,7 +1158,7 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K13" t="n">
         <v>0.25</v>
@@ -1214,7 +1214,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K14" t="n">
         <v>0.25</v>
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="J16" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K16" t="n">
         <v>0.25</v>
@@ -1662,7 +1662,7 @@
         </is>
       </c>
       <c r="J22" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="K22" t="n">
         <v>0.25</v>

</xml_diff>